<commit_message>
Replaced old API with most recent version 37.0 for REST requests
</commit_message>
<xml_diff>
--- a/FailedRecords.xlsx
+++ b/FailedRecords.xlsx
@@ -270,17 +270,17 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>1.9</t>
+          <t/>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2.99</t>
+          <t/>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t/>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -331,24 +331,22 @@
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>Force</t>
+          <t>Suppress</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>123456</t>
+          <t/>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>1. Video Version number is not available in CAS.
-2. Please enter either WS Cost or Price Tier. Not both.
-3. Please enter either Episode Price or Episode Price Tier. Not both.</t>
+          <t>1. Video Version number is not available in CAS.</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t/>
+          <t>Dummy, Title</t>
         </is>
       </c>
     </row>
@@ -411,17 +409,17 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>1.9</t>
+          <t/>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2.99</t>
+          <t/>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t/>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -472,24 +470,22 @@
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>Suppress</t>
+          <t/>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>5678945</t>
+          <t>123</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>1. Video Version number is not available in CAS.
-2. Please enter either WS Cost or Price Tier. Not both.
-3. Please enter either Episode Price or Episode Price Tier. Not both.</t>
+          <t>1. Video Version number is not available in CAS.</t>
         </is>
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t/>
+          <t>Dummy, Title1</t>
         </is>
       </c>
     </row>

</xml_diff>